<commit_message>
Grantt Chart please have look
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfd74915eb265310/Teaching/1810ICT/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chienhuangsarah/Desktop/ST47/SoftwareTechnologyGroup47/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0253012E-9D99-4D40-A479-6A5BC4DCA040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9516"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -24,10 +25,21 @@
     <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$C1,'Project Planner'!$C1+'Project Planner'!$D1-1)</definedName>
     <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
-    <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
+    <definedName name="TitleRegion..BO60">'Project Planner'!$C$3:$C$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,90 +48,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>PERIODS</t>
-  </si>
-  <si>
-    <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -206,65 +137,142 @@
     <t xml:space="preserve"> Period Highlight:</t>
   </si>
   <si>
+    <t>PLAN DURATION</t>
+  </si>
+  <si>
+    <t>ACTUAL START</t>
+  </si>
+  <si>
+    <t>ACTUAL DURATION</t>
+  </si>
+  <si>
+    <t>PERCENT COMPLETE</t>
+  </si>
+  <si>
+    <t>Actual Start</t>
+  </si>
+  <si>
+    <t>Plan Duration</t>
+  </si>
+  <si>
+    <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
+  </si>
+  <si>
+    <t>Activity 33</t>
+  </si>
+  <si>
+    <t>Project Title</t>
+  </si>
+  <si>
+    <t>1.1 Project Background &amp; Overview:</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2 Dataset Analysis &amp; Selection</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.3 Project Scope Definition</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.4 Project Milestone Setting</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.1 Use Case Definition</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2 Use Case In-depth Analysis</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3 User Interaction Requirement Analysis</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.4 Functional Module Division</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5 Prototype &amp; Interface Sketch Design</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.6 Data Structure &amp; Flowchart Design</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.7 UML Modeling &amp; Design</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1 Data Preprocessing &amp; Cleaning</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2 Class &amp; Component Implementation</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3 Algorithm Design &amp; Optimization</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.4 User Interface Development</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.5 API &amp; Method Implementation</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.6 Software Packaging &amp; Test Preparation</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1 Test Plan Design</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2 Internal Testing &amp; Verification</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.3 Test Result Analysis</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.4 Issue Fixing &amp; Optimization</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 Final Software Packaging &amp; Delivery</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1 Project Documentation Writing</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.2 Project Review &amp; Summary</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACTIVITY</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
     <t>PLAN START</t>
-  </si>
-  <si>
-    <t>PLAN DURATION</t>
-  </si>
-  <si>
-    <t>ACTUAL START</t>
-  </si>
-  <si>
-    <t>ACTUAL DURATION</t>
-  </si>
-  <si>
-    <t>PERCENT COMPLETE</t>
-  </si>
-  <si>
-    <t>Actual Start</t>
-  </si>
-  <si>
-    <t>Plan Duration</t>
-  </si>
-  <si>
-    <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
-  </si>
-  <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
-    <t>Activity 34</t>
-  </si>
-  <si>
-    <t>Activity 35</t>
-  </si>
-  <si>
-    <t>Project Title</t>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -364,8 +372,28 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Wawati TC"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Corbel"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +432,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +585,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -582,7 +616,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -618,83 +652,89 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
-    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="一般" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="說明文字" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="標題" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="標題 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="標題 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="標題 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="標題 4" xfId="11" builtinId="19" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="81">
     <dxf>
       <fill>
         <patternFill>
@@ -811,6 +851,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -822,17 +890,884 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
         </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
           <color theme="7"/>
-        </top>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -1189,33 +2124,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO39"/>
+  <dimension ref="A1:CC29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="87" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
-    <col min="42" max="42" width="2.77734375" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="27" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="41" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="2.83203125" customWidth="1"/>
+    <col min="43" max="59" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:81" ht="60" customHeight="1" thickBot="1">
       <c r="B1" s="14" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1223,23 +2162,23 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:81" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="B2" s="24" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="5" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="30" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1247,58 +2186,58 @@
       <c r="O2" s="32"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="30" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="34"/>
+      <c r="V2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AA2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="39"/>
+      <c r="AI2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
     </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>32</v>
+    <row r="3" spans="2:81" s="12" customFormat="1" ht="40" customHeight="1" thickTop="1">
+      <c r="B3" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>39</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>0</v>
@@ -1323,9 +2262,8 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
+    <row r="4" spans="2:81" ht="15.75" customHeight="1">
+      <c r="C4" s="26"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -1510,495 +2448,738 @@
       <c r="BO4" s="3">
         <v>60</v>
       </c>
+      <c r="BP4" s="3">
+        <v>61</v>
+      </c>
+      <c r="BQ4" s="3">
+        <v>62</v>
+      </c>
+      <c r="BR4" s="3">
+        <v>63</v>
+      </c>
+      <c r="BS4" s="3">
+        <v>64</v>
+      </c>
+      <c r="BT4" s="3">
+        <v>65</v>
+      </c>
+      <c r="BU4" s="3">
+        <v>66</v>
+      </c>
+      <c r="BV4" s="3">
+        <v>67</v>
+      </c>
+      <c r="BW4" s="3">
+        <v>68</v>
+      </c>
+      <c r="BX4" s="3">
+        <v>69</v>
+      </c>
+      <c r="BY4" s="3">
+        <v>70</v>
+      </c>
+      <c r="BZ4" s="3">
+        <v>71</v>
+      </c>
+      <c r="CA4" s="3">
+        <v>72</v>
+      </c>
+      <c r="CB4" s="3">
+        <v>73</v>
+      </c>
+      <c r="CC4" s="3">
+        <v>74</v>
+      </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
-        <v>2</v>
+    <row r="5" spans="2:81" ht="30" customHeight="1">
+      <c r="B5" s="37" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
       </c>
       <c r="D5" s="7">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
       <c r="G5" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="2:81" ht="30" customHeight="1">
+      <c r="B6" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="D6" s="7">
+        <v>3</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
       <c r="G6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+    <row r="7" spans="2:81" ht="30" customHeight="1">
+      <c r="B7" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7">
+        <v>2</v>
+      </c>
       <c r="G7" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="2:81" ht="30" customHeight="1">
+      <c r="B8" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
         <v>5</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
       <c r="G8" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:81" ht="30" customHeight="1">
+      <c r="B9" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7">
+        <v>9</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7">
         <v>6</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
       <c r="G9" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+    <row r="10" spans="2:81" ht="30" customHeight="1">
+      <c r="B10" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="7">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7">
+        <v>8</v>
+      </c>
+      <c r="F10" s="7">
+        <v>3</v>
+      </c>
       <c r="G10" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+    <row r="11" spans="2:81" ht="30" customHeight="1">
+      <c r="B11" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="7">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7">
+        <v>11</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3</v>
+      </c>
       <c r="G11" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+    <row r="12" spans="2:81" ht="30" customHeight="1">
+      <c r="B12" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="7">
+        <v>16</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>14</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
       <c r="G12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+    <row r="13" spans="2:81" ht="30" customHeight="1">
+      <c r="B13" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="7">
+        <v>18</v>
+      </c>
+      <c r="D13" s="7">
+        <v>3</v>
+      </c>
+      <c r="E13" s="7">
+        <v>16</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2</v>
+      </c>
       <c r="G13" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+    <row r="14" spans="2:81" ht="30" customHeight="1">
+      <c r="B14" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="7">
+        <v>21</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7">
+        <v>18</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
       <c r="G14" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+    <row r="15" spans="2:81" ht="30" customHeight="1">
+      <c r="B15" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="9">
+        <v>24</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>20</v>
+      </c>
+      <c r="F15" s="7">
+        <v>4</v>
+      </c>
       <c r="G15" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+    <row r="16" spans="2:81" ht="30" customHeight="1">
+      <c r="B16" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="7">
+        <v>28</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+    <row r="17" spans="1:27" ht="30" customHeight="1">
+      <c r="B17" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="7">
+        <v>32</v>
+      </c>
+      <c r="D17" s="7">
+        <v>5</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+    <row r="18" spans="1:27" ht="30" customHeight="1">
+      <c r="B18" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="7">
+        <v>37</v>
+      </c>
+      <c r="D18" s="7">
+        <v>5</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+    <row r="19" spans="1:27" ht="30" customHeight="1">
+      <c r="B19" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="7">
+        <v>42</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+    <row r="20" spans="1:27" ht="30" customHeight="1">
+      <c r="B20" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7">
+        <v>46</v>
+      </c>
+      <c r="D20" s="7">
+        <v>4</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+    <row r="21" spans="1:27" ht="30" customHeight="1">
+      <c r="B21" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="7">
+        <v>50</v>
+      </c>
+      <c r="D21" s="7">
+        <v>2</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+    <row r="22" spans="1:27" ht="30" customHeight="1">
+      <c r="B22" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="7">
+        <v>52</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+    <row r="23" spans="1:27" ht="30" customHeight="1">
+      <c r="B23" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="7">
+        <v>55</v>
+      </c>
+      <c r="D23" s="7">
+        <v>5</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+    <row r="24" spans="1:27" ht="30" customHeight="1">
+      <c r="B24" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="7">
+        <v>60</v>
+      </c>
+      <c r="D24" s="7">
+        <v>2</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+    <row r="25" spans="1:27" ht="30" customHeight="1">
+      <c r="B25" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="7">
+        <v>62</v>
+      </c>
+      <c r="D25" s="7">
+        <v>4</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+    <row r="26" spans="1:27" ht="30" customHeight="1">
+      <c r="B26" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="7">
+        <v>66</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+    <row r="27" spans="1:27" ht="30" customHeight="1">
+      <c r="B27" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="7">
+        <v>68</v>
+      </c>
+      <c r="D27" s="7">
+        <v>4</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+    <row r="28" spans="1:27" ht="30" customHeight="1">
+      <c r="B28" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="7">
+        <v>72</v>
+      </c>
+      <c r="D28" s="7">
+        <v>2</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="6" t="s">
-        <v>26</v>
-      </c>
+    <row r="29" spans="1:27" ht="1" customHeight="1">
+      <c r="A29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="D29" s="7">
+        <v>2</v>
+      </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8">
+      <c r="F29" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8">
-        <v>0</v>
-      </c>
+      <c r="G29" s="1"/>
+      <c r="AA29"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
+  <mergeCells count="10">
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO39">
-    <cfRule type="expression" dxfId="17" priority="1">
+  <phoneticPr fontId="14" type="noConversion"/>
+  <conditionalFormatting sqref="H5:BO28">
+    <cfRule type="expression" dxfId="80" priority="49">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="79" priority="51">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="78" priority="52">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="77" priority="53">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="76" priority="54">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="75" priority="55">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="74" priority="59">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="73" priority="60">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="8" priority="8">
+  <conditionalFormatting sqref="H4:CC4">
+    <cfRule type="expression" dxfId="72" priority="56">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
+  <conditionalFormatting sqref="G29:BN29">
+    <cfRule type="expression" dxfId="71" priority="69">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="70">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="71">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="72">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="73">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="74">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="75">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="76">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BP5:BP28">
+    <cfRule type="expression" dxfId="63" priority="41">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="42">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="43">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="44">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="45">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="46">
+      <formula>BP$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="47">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="48">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ5:BZ28">
+    <cfRule type="expression" dxfId="55" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="30">
+      <formula>BQ$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ29:BY29">
+    <cfRule type="expression" dxfId="47" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="38">
+      <formula>BR$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="40">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CA5:CA28">
+    <cfRule type="expression" dxfId="39" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="22">
+      <formula>CA$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CB5:CB28">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>CB$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CC5:CC28">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>CC$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="15">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
submmit the Gantt chart and Project plan files
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/siqi_wu_griffithuni_edu_au/Documents/7810ICT Software Technologies/Assignment/project/SoftwareTechnologyGroup47/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAAAAAAAcourse\T2\soft-tech\A1\SoftwareTechnologyGroup47\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{0253012E-9D99-4D40-A479-6A5BC4DCA040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC3239EB-05D0-45FB-9156-2585A8A4F9C6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5132A2D1-8DAF-494B-B145-91C52F7C3F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17640" yWindow="3000" windowWidth="28365" windowHeight="16050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -725,12 +725,12 @@
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="标题" xfId="8" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="标题 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="标题 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="解释性文本" xfId="12" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="25">
@@ -983,6 +983,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1077,20 +1091,6 @@
         <bottom style="thin">
           <color theme="0"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -1339,25 +1339,25 @@
   </sheetPr>
   <dimension ref="A1:CC29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AD15" sqref="AD15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="2.88671875" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="33.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16" width="3.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="27" width="4.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="41" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="2.875" customWidth="1"/>
-    <col min="43" max="59" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="67" max="70" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="27" width="4.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="41" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="2.88671875" customWidth="1"/>
+    <col min="43" max="59" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:81" ht="60" customHeight="1" thickBot="1">
@@ -1428,7 +1428,7 @@
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
-    <row r="3" spans="2:81" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
+    <row r="3" spans="2:81" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1">
       <c r="B3" s="28" t="s">
         <v>38</v>
       </c>
@@ -1929,10 +1929,14 @@
       <c r="D16" s="7">
         <v>4</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="E16" s="7">
+        <v>23</v>
+      </c>
+      <c r="F16" s="7">
+        <v>4</v>
+      </c>
       <c r="G16" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="30" customHeight="1">
@@ -1945,10 +1949,14 @@
       <c r="D17" s="7">
         <v>5</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="7">
+        <v>28</v>
+      </c>
+      <c r="F17" s="7">
+        <v>5</v>
+      </c>
       <c r="G17" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="30" customHeight="1">
@@ -1961,10 +1969,14 @@
       <c r="D18" s="7">
         <v>5</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="7">
+        <v>34</v>
+      </c>
+      <c r="F18" s="7">
+        <v>5</v>
+      </c>
       <c r="G18" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="30" customHeight="1">
@@ -1977,10 +1989,14 @@
       <c r="D19" s="7">
         <v>4</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="7">
+        <v>40</v>
+      </c>
+      <c r="F19" s="7">
+        <v>3</v>
+      </c>
       <c r="G19" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="30" customHeight="1">
@@ -1993,10 +2009,14 @@
       <c r="D20" s="7">
         <v>4</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="7">
+        <v>44</v>
+      </c>
+      <c r="F20" s="7">
+        <v>3</v>
+      </c>
       <c r="G20" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="30" customHeight="1">
@@ -2009,10 +2029,14 @@
       <c r="D21" s="7">
         <v>2</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="7">
+        <v>47</v>
+      </c>
+      <c r="F21" s="7">
+        <v>3</v>
+      </c>
       <c r="G21" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="30" customHeight="1">
@@ -2025,10 +2049,14 @@
       <c r="D22" s="7">
         <v>3</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="7">
+        <v>50</v>
+      </c>
+      <c r="F22" s="7">
+        <v>3</v>
+      </c>
       <c r="G22" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="30" customHeight="1">
@@ -2041,10 +2069,14 @@
       <c r="D23" s="7">
         <v>5</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="7">
+        <v>53</v>
+      </c>
+      <c r="F23" s="7">
+        <v>5</v>
+      </c>
       <c r="G23" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="30" customHeight="1">
@@ -2057,10 +2089,14 @@
       <c r="D24" s="7">
         <v>2</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="7">
+        <v>58</v>
+      </c>
+      <c r="F24" s="7">
+        <v>2</v>
+      </c>
       <c r="G24" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="30" customHeight="1">
@@ -2073,10 +2109,14 @@
       <c r="D25" s="7">
         <v>4</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="7">
+        <v>60</v>
+      </c>
+      <c r="F25" s="7">
+        <v>4</v>
+      </c>
       <c r="G25" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="30" customHeight="1">
@@ -2089,10 +2129,14 @@
       <c r="D26" s="7">
         <v>2</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="E26" s="7">
+        <v>64</v>
+      </c>
+      <c r="F26" s="7">
+        <v>3</v>
+      </c>
       <c r="G26" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="30" customHeight="1">
@@ -2105,10 +2149,14 @@
       <c r="D27" s="7">
         <v>4</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="7">
+        <v>67</v>
+      </c>
+      <c r="F27" s="7">
+        <v>4</v>
+      </c>
       <c r="G27" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="30" customHeight="1">
@@ -2121,13 +2169,17 @@
       <c r="D28" s="7">
         <v>2</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="7">
+        <v>71</v>
+      </c>
+      <c r="F28" s="7">
+        <v>2</v>
+      </c>
       <c r="G28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" ht="0.95" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="0.9" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>12</v>
       </c>
@@ -2158,29 +2210,29 @@
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="G29:BN29">
-    <cfRule type="expression" dxfId="24" priority="76">
+    <cfRule type="expression" dxfId="24" priority="69">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="70">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="71">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="72">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="73">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="74">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="75">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="76">
       <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="69">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="70">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="71">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="72">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="73">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="74">
-      <formula>H$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="75">
-      <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:CC4">
@@ -2271,4 +2323,10 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{c9f92db8-2851-4df9-9d12-fab52f5b1415}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>